<commit_message>
Burndown  n Gantt Chart
Update Sprint 4
</commit_message>
<xml_diff>
--- a/Files/BC.xlsx
+++ b/Files/BC.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muham\Desktop\Before Upload Git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muham\Desktop\Before Upload Git\30519\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ALL-Burndown" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
   <si>
     <t>Task</t>
   </si>
@@ -200,6 +200,21 @@
   <si>
     <t>Kuesioner Utama Alumni</t>
   </si>
+  <si>
+    <t>Perbaikan Profil Alumni</t>
+  </si>
+  <si>
+    <t>Perbaikan Kuesioner</t>
+  </si>
+  <si>
+    <t>Perbaikan Tabel Alumni &amp; Admin</t>
+  </si>
+  <si>
+    <t>Fitur Download</t>
+  </si>
+  <si>
+    <t>Fitur Statistik</t>
+  </si>
 </sst>
 </file>
 
@@ -352,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -441,6 +456,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -907,7 +925,7 @@
                   <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1249,136 +1267,136 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="45"/>
                 <c:pt idx="1">
-                  <c:v>308</c:v>
+                  <c:v>288</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0">
-                  <c:v>301.15555555555557</c:v>
+                  <c:v>281.60000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0">
-                  <c:v>294.31111111111113</c:v>
+                  <c:v>275.20000000000005</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0">
-                  <c:v>287.4666666666667</c:v>
+                  <c:v>268.80000000000007</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0">
-                  <c:v>280.62222222222226</c:v>
+                  <c:v>262.40000000000009</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0">
-                  <c:v>273.77777777777783</c:v>
+                  <c:v>256.00000000000011</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0">
-                  <c:v>266.93333333333339</c:v>
+                  <c:v>249.60000000000011</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0">
-                  <c:v>260.08888888888896</c:v>
+                  <c:v>243.2000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0">
-                  <c:v>253.24444444444453</c:v>
+                  <c:v>236.8000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0">
-                  <c:v>246.40000000000009</c:v>
+                  <c:v>230.40000000000009</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0">
-                  <c:v>239.55555555555566</c:v>
+                  <c:v>224.00000000000009</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0">
-                  <c:v>232.71111111111122</c:v>
+                  <c:v>217.60000000000008</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0">
-                  <c:v>225.86666666666679</c:v>
+                  <c:v>211.20000000000007</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0">
-                  <c:v>219.02222222222235</c:v>
+                  <c:v>204.80000000000007</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0">
-                  <c:v>212.17777777777792</c:v>
+                  <c:v>198.40000000000006</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0">
-                  <c:v>205.33333333333348</c:v>
+                  <c:v>192.00000000000006</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0">
-                  <c:v>198.48888888888905</c:v>
+                  <c:v>185.60000000000005</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0">
-                  <c:v>191.64444444444462</c:v>
+                  <c:v>179.20000000000005</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0">
-                  <c:v>184.80000000000018</c:v>
+                  <c:v>172.80000000000004</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0">
-                  <c:v>177.95555555555575</c:v>
+                  <c:v>166.40000000000003</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>171.11111111111131</c:v>
+                  <c:v>160.00000000000003</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0">
-                  <c:v>164.26666666666688</c:v>
+                  <c:v>153.60000000000002</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0">
-                  <c:v>157.42222222222244</c:v>
+                  <c:v>147.20000000000002</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0">
-                  <c:v>150.57777777777801</c:v>
+                  <c:v>140.80000000000001</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0">
-                  <c:v>143.73333333333358</c:v>
+                  <c:v>134.4</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0">
-                  <c:v>136.88888888888914</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0">
-                  <c:v>129.5555555555558</c:v>
+                  <c:v>121.6</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0">
-                  <c:v>122.22222222222247</c:v>
+                  <c:v>115.19999999999999</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0">
-                  <c:v>114.88888888888914</c:v>
+                  <c:v>108.79999999999998</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0">
-                  <c:v>107.55555555555581</c:v>
+                  <c:v>102.39999999999998</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0">
-                  <c:v>100.22222222222248</c:v>
+                  <c:v>95.999999999999972</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0">
-                  <c:v>92.888888888889156</c:v>
+                  <c:v>89.599999999999966</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0">
-                  <c:v>85.555555555555827</c:v>
+                  <c:v>83.19999999999996</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0">
-                  <c:v>78.392764857881403</c:v>
+                  <c:v>76.799999999999955</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0">
-                  <c:v>71.229974160206979</c:v>
+                  <c:v>70.399999999999949</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0">
-                  <c:v>64.067183462532554</c:v>
+                  <c:v>63.99999999999995</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0">
-                  <c:v>56.904392764858137</c:v>
+                  <c:v>57.599999999999952</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0">
-                  <c:v>49.74160206718372</c:v>
+                  <c:v>51.199999999999953</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0">
-                  <c:v>42.578811369509303</c:v>
+                  <c:v>44.799999999999955</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0">
-                  <c:v>35.416020671834886</c:v>
+                  <c:v>38.399999999999956</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0">
-                  <c:v>28.253229974160469</c:v>
+                  <c:v>31.999999999999957</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0">
-                  <c:v>21.090439276486052</c:v>
+                  <c:v>25.599999999999959</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0">
-                  <c:v>13.927648578811633</c:v>
+                  <c:v>19.19999999999996</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0">
-                  <c:v>6.764857881137214</c:v>
+                  <c:v>12.79999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1429,136 +1447,136 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="45"/>
                 <c:pt idx="1">
-                  <c:v>296</c:v>
+                  <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0">
-                  <c:v>294</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0">
-                  <c:v>288</c:v>
+                  <c:v>259</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0">
-                  <c:v>282</c:v>
+                  <c:v>253</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0">
-                  <c:v>276</c:v>
+                  <c:v>247</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0">
-                  <c:v>270</c:v>
+                  <c:v>241</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="0">
-                  <c:v>266</c:v>
+                  <c:v>237</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="0">
-                  <c:v>258</c:v>
+                  <c:v>229</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="0">
-                  <c:v>254</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="10" formatCode="0">
-                  <c:v>250</c:v>
+                  <c:v>221</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0">
-                  <c:v>242</c:v>
+                  <c:v>213</c:v>
                 </c:pt>
                 <c:pt idx="12" formatCode="0">
-                  <c:v>232</c:v>
+                  <c:v>203</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0">
-                  <c:v>228</c:v>
+                  <c:v>199</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0">
-                  <c:v>226</c:v>
+                  <c:v>197</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0">
-                  <c:v>218</c:v>
+                  <c:v>189</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0">
-                  <c:v>212</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0">
-                  <c:v>208</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0">
-                  <c:v>204</c:v>
+                  <c:v>175</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0">
-                  <c:v>200</c:v>
+                  <c:v>171</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0">
-                  <c:v>192</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0">
-                  <c:v>182</c:v>
+                  <c:v>153</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0">
-                  <c:v>172</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0">
-                  <c:v>164</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0">
-                  <c:v>156</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0">
-                  <c:v>152</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0">
-                  <c:v>150</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0">
-                  <c:v>148</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0">
-                  <c:v>146</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0">
-                  <c:v>144</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0">
-                  <c:v>128</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0">
-                  <c:v>116</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0">
-                  <c:v>108</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0">
-                  <c:v>100</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0">
-                  <c:v>90</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0">
-                  <c:v>80</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0">
-                  <c:v>80</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0">
-                  <c:v>80</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0">
-                  <c:v>80</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0">
-                  <c:v>80</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0">
-                  <c:v>80</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0">
-                  <c:v>80</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0">
-                  <c:v>80</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0">
-                  <c:v>80</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0">
-                  <c:v>80</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1780,7 +1798,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1886,7 +1903,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2089,7 +2105,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2379,7 +2394,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2492,7 +2506,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2982,7 +2995,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3091,7 +3103,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3575,7 +3586,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4193,6 +4203,554 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="404987656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint 4</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 4'!$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Estimated Time Remaining (Hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 4'!$E$6:$P$6</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Time (Hour)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24-Apr</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25-Apr</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26-Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27-Apr</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28-Apr</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29-Apr</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30-Apr</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1-May</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2-May</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3-May</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4-May</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 4'!$D$12:$P$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="1">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46.36363636363636</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41.72727272727272</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37.090909090909079</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.454545454545439</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.818181818181802</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23.181818181818166</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.545454545454529</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.909090909090892</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.2727272727272556</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.6363636363636189</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.7763568394002505E-14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F04F-44D9-8751-402628369631}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 4'!$C$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Time Remaining (Hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 4'!$E$6:$P$6</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Time (Hour)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24-Apr</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25-Apr</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26-Apr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27-Apr</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28-Apr</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29-Apr</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30-Apr</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1-May</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2-May</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3-May</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4-May</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 4'!$D$13:$P$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="1">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F04F-44D9-8751-402628369631}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="406520184"/>
+        <c:axId val="406520512"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="406520184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="406520512"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="406520512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="406520184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4523,6 +5081,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="294">
   <cs:axisTitle>
@@ -7115,6 +7713,502 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7795,6 +8889,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1568823</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>107576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>302559</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>156882</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -8075,10 +9204,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D6:AX30"/>
+  <dimension ref="D6:AZ30"/>
   <sheetViews>
-    <sheetView topLeftCell="G10" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="T30" sqref="T30"/>
+    <sheetView topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AZ28" sqref="AZ28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8087,15 +9216,16 @@
     <col min="5" max="5" width="23.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="16" width="11.42578125" customWidth="1"/>
+    <col min="52" max="52" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="27"/>
       <c r="H6" s="27"/>
       <c r="I6" s="27"/>
@@ -8199,7 +9329,7 @@
         <v>60</v>
       </c>
       <c r="F11" s="10">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="G11" s="18"/>
       <c r="H11" s="18"/>
@@ -8236,13 +9366,13 @@
       <c r="O15" s="24"/>
       <c r="P15" s="24"/>
     </row>
-    <row r="22" spans="4:50" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:52" x14ac:dyDescent="0.25">
       <c r="G22">
         <f>E14-($E$14/14)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:50" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:52" x14ac:dyDescent="0.25">
       <c r="D23" s="1" t="s">
         <v>1</v>
       </c>
@@ -8355,19 +9485,19 @@
         <v>43575</v>
       </c>
       <c r="AO23" s="29">
-        <v>43577</v>
+        <v>43579</v>
       </c>
       <c r="AP23" s="29">
-        <v>43578</v>
+        <v>43580</v>
       </c>
       <c r="AQ23" s="29">
-        <v>43579</v>
+        <v>43581</v>
       </c>
       <c r="AR23" s="29">
-        <v>43580</v>
+        <v>43582</v>
       </c>
       <c r="AS23" s="29">
-        <v>43581</v>
+        <v>43583</v>
       </c>
       <c r="AT23" s="29">
         <v>43584</v>
@@ -8381,11 +9511,17 @@
       <c r="AW23" s="29">
         <v>43587</v>
       </c>
-      <c r="AX23" s="1" t="s">
+      <c r="AX23" s="29">
+        <v>43588</v>
+      </c>
+      <c r="AY23" s="29">
+        <v>43589</v>
+      </c>
+      <c r="AZ23" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="4:50" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:52" x14ac:dyDescent="0.25">
       <c r="D24" s="14">
         <v>1</v>
       </c>
@@ -8524,11 +9660,17 @@
       <c r="AW24" s="32">
         <v>0</v>
       </c>
-      <c r="AX24" s="30">
+      <c r="AX24" s="32">
+        <v>0</v>
+      </c>
+      <c r="AY24" s="32">
+        <v>0</v>
+      </c>
+      <c r="AZ24" s="30">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="4:50" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:52" x14ac:dyDescent="0.25">
       <c r="D25" s="14">
         <v>2</v>
       </c>
@@ -8667,11 +9809,17 @@
       <c r="AW25" s="32">
         <v>0</v>
       </c>
-      <c r="AX25" s="30">
+      <c r="AX25" s="32">
+        <v>0</v>
+      </c>
+      <c r="AY25" s="32">
+        <v>0</v>
+      </c>
+      <c r="AZ25" s="30">
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="4:50" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:52" x14ac:dyDescent="0.25">
       <c r="D26" s="14">
         <v>3</v>
       </c>
@@ -8810,11 +9958,17 @@
       <c r="AW26" s="32">
         <v>0</v>
       </c>
-      <c r="AX26" s="30">
+      <c r="AX26" s="32">
+        <v>0</v>
+      </c>
+      <c r="AY26" s="32">
+        <v>0</v>
+      </c>
+      <c r="AZ26" s="30">
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="4:50" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:52" x14ac:dyDescent="0.25">
       <c r="D27" s="14">
         <v>4</v>
       </c>
@@ -8822,7 +9976,7 @@
         <v>42</v>
       </c>
       <c r="F27" s="30">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="G27" s="31">
         <v>0</v>
@@ -8953,16 +10107,22 @@
       <c r="AW27" s="32">
         <v>0</v>
       </c>
-      <c r="AX27" s="30">
-        <v>80</v>
+      <c r="AX27" s="32">
+        <v>0</v>
+      </c>
+      <c r="AY27" s="32">
+        <v>0</v>
+      </c>
+      <c r="AZ27" s="30">
+        <v>51</v>
       </c>
     </row>
-    <row r="28" spans="4:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D28" s="37" t="s">
+    <row r="28" spans="4:52" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
       <c r="G28" s="31">
         <f>SUM(G24:G27)</f>
         <v>2</v>
@@ -9100,405 +10260,418 @@
         <v>10</v>
       </c>
       <c r="AO28" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP28" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AQ28" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AR28" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AS28" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AT28" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AU28" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AV28" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AW28" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AX28" s="34"/>
+        <v>4</v>
+      </c>
+      <c r="AX28" s="31">
+        <v>4</v>
+      </c>
+      <c r="AY28" s="31">
+        <v>4</v>
+      </c>
+      <c r="AZ28" s="34"/>
     </row>
-    <row r="29" spans="4:50" x14ac:dyDescent="0.25">
-      <c r="D29" s="36" t="s">
+    <row r="29" spans="4:52" x14ac:dyDescent="0.25">
+      <c r="D29" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="36"/>
+      <c r="E29" s="37"/>
       <c r="F29" s="12">
         <f>SUM(F24:F27)</f>
-        <v>308</v>
+        <v>288</v>
       </c>
       <c r="G29" s="33">
         <f>F29-($F$29/45)</f>
-        <v>301.15555555555557</v>
+        <v>281.60000000000002</v>
       </c>
       <c r="H29" s="33">
-        <f>G29-($F$29/45)</f>
-        <v>294.31111111111113</v>
+        <f t="shared" ref="H29:AY29" si="1">G29-($F$29/45)</f>
+        <v>275.20000000000005</v>
       </c>
       <c r="I29" s="33">
-        <f>H29-($F$29/45)</f>
-        <v>287.4666666666667</v>
+        <f t="shared" si="1"/>
+        <v>268.80000000000007</v>
       </c>
       <c r="J29" s="33">
-        <f t="shared" ref="J29:AE29" si="1">I29-($F$29/45)</f>
-        <v>280.62222222222226</v>
+        <f t="shared" si="1"/>
+        <v>262.40000000000009</v>
       </c>
       <c r="K29" s="33">
         <f t="shared" si="1"/>
-        <v>273.77777777777783</v>
+        <v>256.00000000000011</v>
       </c>
       <c r="L29" s="33">
         <f t="shared" si="1"/>
-        <v>266.93333333333339</v>
+        <v>249.60000000000011</v>
       </c>
       <c r="M29" s="33">
         <f t="shared" si="1"/>
-        <v>260.08888888888896</v>
+        <v>243.2000000000001</v>
       </c>
       <c r="N29" s="33">
         <f t="shared" si="1"/>
-        <v>253.24444444444453</v>
+        <v>236.8000000000001</v>
       </c>
       <c r="O29" s="33">
         <f t="shared" si="1"/>
-        <v>246.40000000000009</v>
+        <v>230.40000000000009</v>
       </c>
       <c r="P29" s="33">
         <f t="shared" si="1"/>
-        <v>239.55555555555566</v>
+        <v>224.00000000000009</v>
       </c>
       <c r="Q29" s="33">
         <f t="shared" si="1"/>
-        <v>232.71111111111122</v>
+        <v>217.60000000000008</v>
       </c>
       <c r="R29" s="33">
         <f t="shared" si="1"/>
-        <v>225.86666666666679</v>
+        <v>211.20000000000007</v>
       </c>
       <c r="S29" s="33">
         <f t="shared" si="1"/>
-        <v>219.02222222222235</v>
+        <v>204.80000000000007</v>
       </c>
       <c r="T29" s="33">
         <f t="shared" si="1"/>
-        <v>212.17777777777792</v>
+        <v>198.40000000000006</v>
       </c>
       <c r="U29" s="33">
         <f t="shared" si="1"/>
-        <v>205.33333333333348</v>
+        <v>192.00000000000006</v>
       </c>
       <c r="V29" s="33">
         <f t="shared" si="1"/>
-        <v>198.48888888888905</v>
+        <v>185.60000000000005</v>
       </c>
       <c r="W29" s="33">
         <f t="shared" si="1"/>
-        <v>191.64444444444462</v>
+        <v>179.20000000000005</v>
       </c>
       <c r="X29" s="33">
         <f t="shared" si="1"/>
-        <v>184.80000000000018</v>
+        <v>172.80000000000004</v>
       </c>
       <c r="Y29" s="33">
         <f t="shared" si="1"/>
-        <v>177.95555555555575</v>
+        <v>166.40000000000003</v>
       </c>
       <c r="Z29" s="33">
         <f t="shared" si="1"/>
-        <v>171.11111111111131</v>
+        <v>160.00000000000003</v>
       </c>
       <c r="AA29" s="33">
         <f t="shared" si="1"/>
-        <v>164.26666666666688</v>
+        <v>153.60000000000002</v>
       </c>
       <c r="AB29" s="33">
         <f t="shared" si="1"/>
-        <v>157.42222222222244</v>
+        <v>147.20000000000002</v>
       </c>
       <c r="AC29" s="33">
         <f t="shared" si="1"/>
-        <v>150.57777777777801</v>
+        <v>140.80000000000001</v>
       </c>
       <c r="AD29" s="33">
         <f t="shared" si="1"/>
-        <v>143.73333333333358</v>
+        <v>134.4</v>
       </c>
       <c r="AE29" s="33">
         <f t="shared" si="1"/>
-        <v>136.88888888888914</v>
+        <v>128</v>
       </c>
       <c r="AF29" s="33">
-        <f>AE29-($F$29/42)</f>
-        <v>129.5555555555558</v>
+        <f t="shared" si="1"/>
+        <v>121.6</v>
       </c>
       <c r="AG29" s="33">
-        <f t="shared" ref="AG29:AW29" si="2">AF29-($F$29/42)</f>
-        <v>122.22222222222247</v>
+        <f t="shared" si="1"/>
+        <v>115.19999999999999</v>
       </c>
       <c r="AH29" s="33">
-        <f t="shared" si="2"/>
-        <v>114.88888888888914</v>
+        <f t="shared" si="1"/>
+        <v>108.79999999999998</v>
       </c>
       <c r="AI29" s="33">
-        <f t="shared" si="2"/>
-        <v>107.55555555555581</v>
+        <f t="shared" si="1"/>
+        <v>102.39999999999998</v>
       </c>
       <c r="AJ29" s="33">
-        <f t="shared" si="2"/>
-        <v>100.22222222222248</v>
+        <f t="shared" si="1"/>
+        <v>95.999999999999972</v>
       </c>
       <c r="AK29" s="33">
-        <f t="shared" si="2"/>
-        <v>92.888888888889156</v>
+        <f t="shared" si="1"/>
+        <v>89.599999999999966</v>
       </c>
       <c r="AL29" s="33">
-        <f t="shared" si="2"/>
-        <v>85.555555555555827</v>
+        <f t="shared" si="1"/>
+        <v>83.19999999999996</v>
       </c>
       <c r="AM29" s="33">
-        <f>AL29-($F$29/43)</f>
-        <v>78.392764857881403</v>
+        <f t="shared" si="1"/>
+        <v>76.799999999999955</v>
       </c>
       <c r="AN29" s="33">
-        <f t="shared" ref="AN29:AW29" si="3">AM29-($F$29/43)</f>
-        <v>71.229974160206979</v>
+        <f t="shared" si="1"/>
+        <v>70.399999999999949</v>
       </c>
       <c r="AO29" s="33">
-        <f t="shared" si="3"/>
-        <v>64.067183462532554</v>
+        <f t="shared" si="1"/>
+        <v>63.99999999999995</v>
       </c>
       <c r="AP29" s="33">
-        <f t="shared" si="3"/>
-        <v>56.904392764858137</v>
+        <f t="shared" si="1"/>
+        <v>57.599999999999952</v>
       </c>
       <c r="AQ29" s="33">
-        <f t="shared" si="3"/>
-        <v>49.74160206718372</v>
+        <f t="shared" si="1"/>
+        <v>51.199999999999953</v>
       </c>
       <c r="AR29" s="33">
-        <f t="shared" si="3"/>
-        <v>42.578811369509303</v>
+        <f t="shared" si="1"/>
+        <v>44.799999999999955</v>
       </c>
       <c r="AS29" s="33">
-        <f t="shared" si="3"/>
-        <v>35.416020671834886</v>
+        <f t="shared" si="1"/>
+        <v>38.399999999999956</v>
       </c>
       <c r="AT29" s="33">
-        <f t="shared" si="3"/>
-        <v>28.253229974160469</v>
+        <f t="shared" si="1"/>
+        <v>31.999999999999957</v>
       </c>
       <c r="AU29" s="33">
-        <f t="shared" si="3"/>
-        <v>21.090439276486052</v>
+        <f t="shared" si="1"/>
+        <v>25.599999999999959</v>
       </c>
       <c r="AV29" s="33">
-        <f t="shared" si="3"/>
-        <v>13.927648578811633</v>
+        <f t="shared" si="1"/>
+        <v>19.19999999999996</v>
       </c>
       <c r="AW29" s="33">
-        <f t="shared" si="3"/>
-        <v>6.764857881137214</v>
+        <f t="shared" si="1"/>
+        <v>12.79999999999996</v>
+      </c>
+      <c r="AX29" s="33">
+        <f t="shared" si="1"/>
+        <v>6.3999999999999595</v>
+      </c>
+      <c r="AY29" s="33">
+        <f t="shared" si="1"/>
+        <v>-4.0856207306205761E-14</v>
       </c>
     </row>
-    <row r="30" spans="4:50" x14ac:dyDescent="0.25">
-      <c r="D30" s="36" t="s">
+    <row r="30" spans="4:52" x14ac:dyDescent="0.25">
+      <c r="D30" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="E30" s="36"/>
+      <c r="E30" s="37"/>
       <c r="F30" s="12">
-        <f>SUM(AX24:AX27)</f>
-        <v>296</v>
+        <f>SUM(AZ24:AZ27)</f>
+        <v>267</v>
       </c>
       <c r="G30" s="33">
         <f>SUM(F30-G28)</f>
-        <v>294</v>
+        <v>265</v>
       </c>
       <c r="H30" s="33">
-        <f>SUM(G30-H28)</f>
-        <v>288</v>
+        <f t="shared" ref="H30:AY30" si="2">SUM(G30-H28)</f>
+        <v>259</v>
       </c>
       <c r="I30" s="33">
-        <f>SUM(H30-I28)</f>
-        <v>282</v>
+        <f t="shared" si="2"/>
+        <v>253</v>
       </c>
       <c r="J30" s="33">
-        <f t="shared" ref="J30:AF30" si="4">SUM(I30-J28)</f>
-        <v>276</v>
+        <f t="shared" si="2"/>
+        <v>247</v>
       </c>
       <c r="K30" s="33">
-        <f t="shared" si="4"/>
-        <v>270</v>
+        <f t="shared" si="2"/>
+        <v>241</v>
       </c>
       <c r="L30" s="33">
-        <f t="shared" si="4"/>
-        <v>266</v>
+        <f t="shared" si="2"/>
+        <v>237</v>
       </c>
       <c r="M30" s="33">
-        <f t="shared" si="4"/>
-        <v>258</v>
+        <f t="shared" si="2"/>
+        <v>229</v>
       </c>
       <c r="N30" s="33">
-        <f t="shared" si="4"/>
-        <v>254</v>
+        <f t="shared" si="2"/>
+        <v>225</v>
       </c>
       <c r="O30" s="33">
-        <f t="shared" si="4"/>
-        <v>250</v>
+        <f t="shared" si="2"/>
+        <v>221</v>
       </c>
       <c r="P30" s="33">
-        <f t="shared" si="4"/>
-        <v>242</v>
+        <f t="shared" si="2"/>
+        <v>213</v>
       </c>
       <c r="Q30" s="33">
-        <f t="shared" si="4"/>
-        <v>232</v>
+        <f t="shared" si="2"/>
+        <v>203</v>
       </c>
       <c r="R30" s="33">
-        <f t="shared" si="4"/>
-        <v>228</v>
+        <f t="shared" si="2"/>
+        <v>199</v>
       </c>
       <c r="S30" s="33">
-        <f t="shared" si="4"/>
-        <v>226</v>
+        <f t="shared" si="2"/>
+        <v>197</v>
       </c>
       <c r="T30" s="33">
-        <f t="shared" si="4"/>
-        <v>218</v>
+        <f t="shared" si="2"/>
+        <v>189</v>
       </c>
       <c r="U30" s="33">
-        <f t="shared" si="4"/>
-        <v>212</v>
+        <f t="shared" si="2"/>
+        <v>183</v>
       </c>
       <c r="V30" s="33">
-        <f t="shared" si="4"/>
-        <v>208</v>
+        <f t="shared" si="2"/>
+        <v>179</v>
       </c>
       <c r="W30" s="33">
-        <f t="shared" si="4"/>
-        <v>204</v>
+        <f t="shared" si="2"/>
+        <v>175</v>
       </c>
       <c r="X30" s="33">
-        <f t="shared" si="4"/>
-        <v>200</v>
+        <f t="shared" si="2"/>
+        <v>171</v>
       </c>
       <c r="Y30" s="33">
-        <f t="shared" si="4"/>
-        <v>192</v>
+        <f t="shared" si="2"/>
+        <v>163</v>
       </c>
       <c r="Z30" s="33">
-        <f t="shared" si="4"/>
-        <v>182</v>
+        <f t="shared" si="2"/>
+        <v>153</v>
       </c>
       <c r="AA30" s="33">
-        <f t="shared" si="4"/>
-        <v>172</v>
+        <f t="shared" si="2"/>
+        <v>143</v>
       </c>
       <c r="AB30" s="33">
-        <f t="shared" si="4"/>
-        <v>164</v>
+        <f t="shared" si="2"/>
+        <v>135</v>
       </c>
       <c r="AC30" s="33">
-        <f t="shared" si="4"/>
-        <v>156</v>
+        <f t="shared" si="2"/>
+        <v>127</v>
       </c>
       <c r="AD30" s="33">
-        <f t="shared" si="4"/>
-        <v>152</v>
+        <f t="shared" si="2"/>
+        <v>123</v>
       </c>
       <c r="AE30" s="33">
-        <f t="shared" si="4"/>
-        <v>150</v>
+        <f t="shared" si="2"/>
+        <v>121</v>
       </c>
       <c r="AF30" s="33">
-        <f t="shared" si="4"/>
-        <v>148</v>
+        <f t="shared" si="2"/>
+        <v>119</v>
       </c>
       <c r="AG30" s="33">
-        <f t="shared" ref="AG30" si="5">SUM(AF30-AG28)</f>
-        <v>146</v>
+        <f t="shared" si="2"/>
+        <v>117</v>
       </c>
       <c r="AH30" s="33">
-        <f t="shared" ref="AH30" si="6">SUM(AG30-AH28)</f>
-        <v>144</v>
+        <f t="shared" si="2"/>
+        <v>115</v>
       </c>
       <c r="AI30" s="33">
-        <f t="shared" ref="AI30" si="7">SUM(AH30-AI28)</f>
-        <v>128</v>
+        <f t="shared" si="2"/>
+        <v>99</v>
       </c>
       <c r="AJ30" s="33">
-        <f t="shared" ref="AJ30" si="8">SUM(AI30-AJ28)</f>
-        <v>116</v>
+        <f t="shared" si="2"/>
+        <v>87</v>
       </c>
       <c r="AK30" s="33">
-        <f t="shared" ref="AK30" si="9">SUM(AJ30-AK28)</f>
-        <v>108</v>
+        <f t="shared" si="2"/>
+        <v>79</v>
       </c>
       <c r="AL30" s="33">
-        <f t="shared" ref="AL30" si="10">SUM(AK30-AL28)</f>
-        <v>100</v>
+        <f t="shared" si="2"/>
+        <v>71</v>
       </c>
       <c r="AM30" s="33">
-        <f t="shared" ref="AM30" si="11">SUM(AL30-AM28)</f>
-        <v>90</v>
+        <f t="shared" si="2"/>
+        <v>61</v>
       </c>
       <c r="AN30" s="33">
-        <f t="shared" ref="AN30" si="12">SUM(AM30-AN28)</f>
-        <v>80</v>
+        <f t="shared" si="2"/>
+        <v>51</v>
       </c>
       <c r="AO30" s="33">
-        <f t="shared" ref="AO30" si="13">SUM(AN30-AO28)</f>
-        <v>80</v>
+        <f t="shared" si="2"/>
+        <v>49</v>
       </c>
       <c r="AP30" s="33">
-        <f t="shared" ref="AP30" si="14">SUM(AO30-AP28)</f>
-        <v>80</v>
+        <f t="shared" si="2"/>
+        <v>46</v>
       </c>
       <c r="AQ30" s="33">
-        <f t="shared" ref="AQ30" si="15">SUM(AP30-AQ28)</f>
-        <v>80</v>
+        <f t="shared" si="2"/>
+        <v>42</v>
       </c>
       <c r="AR30" s="33">
-        <f t="shared" ref="AR30" si="16">SUM(AQ30-AR28)</f>
-        <v>80</v>
+        <f t="shared" si="2"/>
+        <v>36</v>
       </c>
       <c r="AS30" s="33">
-        <f t="shared" ref="AS30" si="17">SUM(AR30-AS28)</f>
-        <v>80</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="AT30" s="33">
-        <f t="shared" ref="AT30" si="18">SUM(AS30-AT28)</f>
-        <v>80</v>
+        <f t="shared" si="2"/>
+        <v>25</v>
       </c>
       <c r="AU30" s="33">
-        <f t="shared" ref="AU30" si="19">SUM(AT30-AU28)</f>
-        <v>80</v>
+        <f t="shared" si="2"/>
+        <v>18</v>
       </c>
       <c r="AV30" s="33">
-        <f t="shared" ref="AV30" si="20">SUM(AU30-AV28)</f>
-        <v>80</v>
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="AW30" s="33">
-        <f t="shared" ref="AW30" si="21">SUM(AV30-AW28)</f>
-        <v>80</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="AX30" s="33">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AY30" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -9850,10 +11023,10 @@
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="36"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="7">
         <f>SUM(D7:D11)</f>
         <v>68</v>
@@ -9916,10 +11089,10 @@
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="36"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="7">
         <f>SUM(D7:D11)</f>
         <v>68</v>
@@ -10488,10 +11661,10 @@
       </c>
     </row>
     <row r="14" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="36"/>
+      <c r="D14" s="37"/>
       <c r="E14" s="8">
         <f>SUM(E6:E13)</f>
         <v>80</v>
@@ -10554,10 +11727,10 @@
       </c>
     </row>
     <row r="15" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="36"/>
+      <c r="D15" s="37"/>
       <c r="E15" s="8">
         <f>SUM(E6:E13)</f>
         <v>80</v>
@@ -10633,8 +11806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11085,10 +12258,10 @@
       </c>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="36"/>
+      <c r="D16" s="37"/>
       <c r="E16" s="17">
         <f>SUM(E7:E15)</f>
         <v>72</v>
@@ -11139,10 +12312,10 @@
       </c>
     </row>
     <row r="17" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="36"/>
+      <c r="D17" s="37"/>
       <c r="E17" s="17">
         <f>SUM(E7:E15)</f>
         <v>72</v>
@@ -11204,12 +12377,396 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C6:P13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="15">
+        <v>43579</v>
+      </c>
+      <c r="G6" s="15">
+        <v>43580</v>
+      </c>
+      <c r="H6" s="15">
+        <v>43581</v>
+      </c>
+      <c r="I6" s="15">
+        <v>43582</v>
+      </c>
+      <c r="J6" s="15">
+        <v>43583</v>
+      </c>
+      <c r="K6" s="15">
+        <v>43584</v>
+      </c>
+      <c r="L6" s="15">
+        <v>43585</v>
+      </c>
+      <c r="M6" s="15">
+        <v>43586</v>
+      </c>
+      <c r="N6" s="15">
+        <v>43587</v>
+      </c>
+      <c r="O6" s="15">
+        <v>43588</v>
+      </c>
+      <c r="P6" s="15">
+        <v>43589</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C7" s="14">
+        <v>1</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="4">
+        <v>6</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <v>1</v>
+      </c>
+      <c r="H7" s="9">
+        <v>1</v>
+      </c>
+      <c r="I7" s="9">
+        <v>1</v>
+      </c>
+      <c r="J7" s="9">
+        <v>3</v>
+      </c>
+      <c r="K7" s="9">
+        <v>0</v>
+      </c>
+      <c r="L7" s="9">
+        <v>0</v>
+      </c>
+      <c r="M7" s="10">
+        <v>0</v>
+      </c>
+      <c r="N7" s="10">
+        <v>0</v>
+      </c>
+      <c r="O7" s="10">
+        <v>0</v>
+      </c>
+      <c r="P7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C8" s="14">
+        <v>2</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="4">
+        <v>6</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="9">
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
+        <v>1</v>
+      </c>
+      <c r="J8" s="9">
+        <v>1</v>
+      </c>
+      <c r="K8" s="9">
+        <v>3</v>
+      </c>
+      <c r="L8" s="9">
+        <v>0</v>
+      </c>
+      <c r="M8" s="10">
+        <v>0</v>
+      </c>
+      <c r="N8" s="10">
+        <v>0</v>
+      </c>
+      <c r="O8" s="10">
+        <v>0</v>
+      </c>
+      <c r="P8" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C9" s="14">
+        <v>3</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="4">
+        <v>7</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="9">
+        <v>1</v>
+      </c>
+      <c r="J9" s="9">
+        <v>1</v>
+      </c>
+      <c r="K9" s="9">
+        <v>2</v>
+      </c>
+      <c r="L9" s="9">
+        <v>3</v>
+      </c>
+      <c r="M9" s="10">
+        <v>0</v>
+      </c>
+      <c r="N9" s="10">
+        <v>0</v>
+      </c>
+      <c r="O9" s="10">
+        <v>0</v>
+      </c>
+      <c r="P9" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C10" s="14">
+        <v>4</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="4">
+        <v>16</v>
+      </c>
+      <c r="F10" s="9">
+        <v>2</v>
+      </c>
+      <c r="G10" s="9">
+        <v>2</v>
+      </c>
+      <c r="H10" s="9">
+        <v>2</v>
+      </c>
+      <c r="I10" s="9">
+        <v>2</v>
+      </c>
+      <c r="J10" s="9">
+        <v>0</v>
+      </c>
+      <c r="K10" s="9">
+        <v>0</v>
+      </c>
+      <c r="L10" s="9">
+        <v>4</v>
+      </c>
+      <c r="M10" s="10">
+        <v>4</v>
+      </c>
+      <c r="N10" s="10">
+        <v>0</v>
+      </c>
+      <c r="O10" s="10">
+        <v>0</v>
+      </c>
+      <c r="P10" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C11" s="14">
+        <v>5</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="5">
+        <v>16</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9">
+        <v>0</v>
+      </c>
+      <c r="I11" s="9">
+        <v>1</v>
+      </c>
+      <c r="J11" s="9">
+        <v>1</v>
+      </c>
+      <c r="K11" s="9">
+        <v>0</v>
+      </c>
+      <c r="L11" s="9">
+        <v>0</v>
+      </c>
+      <c r="M11" s="10">
+        <v>2</v>
+      </c>
+      <c r="N11" s="10">
+        <v>4</v>
+      </c>
+      <c r="O11" s="10">
+        <v>4</v>
+      </c>
+      <c r="P11" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C12" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="37"/>
+      <c r="E12" s="35">
+        <f>SUM(E7:E11)</f>
+        <v>51</v>
+      </c>
+      <c r="F12" s="35">
+        <f>E12-($E$12/11)</f>
+        <v>46.36363636363636</v>
+      </c>
+      <c r="G12" s="35">
+        <f t="shared" ref="G12:P12" si="0">F12-($E$12/11)</f>
+        <v>41.72727272727272</v>
+      </c>
+      <c r="H12" s="35">
+        <f t="shared" si="0"/>
+        <v>37.090909090909079</v>
+      </c>
+      <c r="I12" s="35">
+        <f t="shared" si="0"/>
+        <v>32.454545454545439</v>
+      </c>
+      <c r="J12" s="35">
+        <f t="shared" si="0"/>
+        <v>27.818181818181802</v>
+      </c>
+      <c r="K12" s="35">
+        <f t="shared" si="0"/>
+        <v>23.181818181818166</v>
+      </c>
+      <c r="L12" s="35">
+        <f t="shared" si="0"/>
+        <v>18.545454545454529</v>
+      </c>
+      <c r="M12" s="35">
+        <f t="shared" si="0"/>
+        <v>13.909090909090892</v>
+      </c>
+      <c r="N12" s="35">
+        <f t="shared" si="0"/>
+        <v>9.2727272727272556</v>
+      </c>
+      <c r="O12" s="35">
+        <f t="shared" si="0"/>
+        <v>4.6363636363636189</v>
+      </c>
+      <c r="P12" s="35">
+        <f t="shared" si="0"/>
+        <v>-1.7763568394002505E-14</v>
+      </c>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C13" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="37"/>
+      <c r="E13" s="35">
+        <f>SUM(E7:E11)</f>
+        <v>51</v>
+      </c>
+      <c r="F13" s="35">
+        <f>E13-SUM(F7:F11)</f>
+        <v>49</v>
+      </c>
+      <c r="G13" s="35">
+        <f>F13-SUM(G7:G11)</f>
+        <v>46</v>
+      </c>
+      <c r="H13" s="35">
+        <f>G13-SUM(H7:H11)</f>
+        <v>42</v>
+      </c>
+      <c r="I13" s="35">
+        <f>H13-SUM(I7:I11)</f>
+        <v>36</v>
+      </c>
+      <c r="J13" s="35">
+        <f>I13-SUM(J7:J11)</f>
+        <v>30</v>
+      </c>
+      <c r="K13" s="35">
+        <f>J13-SUM(K7:K11)</f>
+        <v>25</v>
+      </c>
+      <c r="L13" s="35">
+        <f>K13-SUM(L7:L11)</f>
+        <v>18</v>
+      </c>
+      <c r="M13" s="35">
+        <f>L13-SUM(M7:M11)</f>
+        <v>12</v>
+      </c>
+      <c r="N13" s="35">
+        <f>M13-SUM(N7:N11)</f>
+        <v>8</v>
+      </c>
+      <c r="O13" s="35">
+        <f>N13-SUM(O7:O11)</f>
+        <v>4</v>
+      </c>
+      <c r="P13" s="35">
+        <f>O13-SUM(P7:P11)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>